<commit_message>
FEAT-DATA01: actualizar archivo all_fields.xlsx con nuevos datos
</commit_message>
<xml_diff>
--- a/all_fields.xlsx
+++ b/all_fields.xlsx
@@ -1143,7 +1143,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>TTipoPresuntoDelito</t>
+          <t>TInstitucionDemanda</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1158,7 +1158,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>TTipoPresuntoDelito</t>
+          <t>TInstitucionDemanda</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1178,41 +1178,41 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>tipo_institucion</t>
         </is>
       </c>
       <c r="C50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>TInstitucionDemanda</t>
+          <t>TDemanda</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>TInstitucionDemanda</t>
+          <t>TDemanda</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>tipo_institucion</t>
+          <t>fecha_creacion</t>
         </is>
       </c>
       <c r="C52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>ultima_actualizacion</t>
         </is>
       </c>
       <c r="C53" t="b">
@@ -1238,11 +1238,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>fecha_creacion</t>
+          <t>fecha_ingreso_senaf</t>
         </is>
       </c>
       <c r="C54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -1253,11 +1253,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>ultima_actualizacion</t>
+          <t>fecha_oficio_documento</t>
         </is>
       </c>
       <c r="C55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -1268,11 +1268,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>fecha_ingreso_senaf</t>
+          <t>descripcion</t>
         </is>
       </c>
       <c r="C56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1283,11 +1283,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>fecha_oficio_documento</t>
+          <t>objetivo_de_demanda</t>
         </is>
       </c>
       <c r="C57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1298,7 +1298,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>descripcion</t>
+          <t>estado_demanda</t>
         </is>
       </c>
       <c r="C58" t="b">
@@ -1313,11 +1313,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>objetivo_de_demanda</t>
+          <t>observaciones</t>
         </is>
       </c>
       <c r="C59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>estado_demanda</t>
+          <t>envio_de_respuesta</t>
         </is>
       </c>
       <c r="C60" t="b">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>observaciones</t>
+          <t>etiqueta</t>
         </is>
       </c>
       <c r="C61" t="b">
@@ -1358,7 +1358,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>tipo_demanda</t>
+          <t>localizacion</t>
         </is>
       </c>
       <c r="C62" t="b">
@@ -1373,11 +1373,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>localizacion</t>
+          <t>ambito_vulneracion</t>
         </is>
       </c>
       <c r="C63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -1388,11 +1388,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>ambito_vulneracion</t>
+          <t>bloque_datos_remitente</t>
         </is>
       </c>
       <c r="C64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>tipos_presuntos_delitos</t>
+          <t>tipo_institucion</t>
         </is>
       </c>
       <c r="C65" t="b">
@@ -1418,11 +1418,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>bloque_datos_remitente</t>
+          <t>institucion</t>
         </is>
       </c>
       <c r="C66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -1433,7 +1433,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>tipo_institucion</t>
+          <t>motivo_ingreso</t>
         </is>
       </c>
       <c r="C67" t="b">
@@ -1448,7 +1448,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>institucion</t>
+          <t>submotivo_ingreso</t>
         </is>
       </c>
       <c r="C68" t="b">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>motivo_ingreso</t>
+          <t>registrado_por_user</t>
         </is>
       </c>
       <c r="C69" t="b">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>submotivo_ingreso</t>
+          <t>registrado_por_user_zona</t>
         </is>
       </c>
       <c r="C70" t="b">
@@ -1488,12 +1488,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>TDemanda</t>
+          <t>TDemandaHistory</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>registrado_por_user</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C71" t="b">
@@ -1503,16 +1503,16 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>TDemanda</t>
+          <t>TDemandaHistory</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>registrado_por_user_zona</t>
+          <t>action</t>
         </is>
       </c>
       <c r="C72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>by_user</t>
         </is>
       </c>
       <c r="C73" t="b">
@@ -1538,11 +1538,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>action</t>
+          <t>timestamp</t>
         </is>
       </c>
       <c r="C74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>by_user</t>
+          <t>fecha_creacion</t>
         </is>
       </c>
       <c r="C75" t="b">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>timestamp</t>
+          <t>ultima_actualizacion</t>
         </is>
       </c>
       <c r="C76" t="b">
@@ -1583,11 +1583,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>fecha_creacion</t>
+          <t>fecha_ingreso_senaf</t>
         </is>
       </c>
       <c r="C77" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -1598,11 +1598,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>ultima_actualizacion</t>
+          <t>fecha_oficio_documento</t>
         </is>
       </c>
       <c r="C78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -1613,11 +1613,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>fecha_ingreso_senaf</t>
+          <t>descripcion</t>
         </is>
       </c>
       <c r="C79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -1628,11 +1628,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>fecha_oficio_documento</t>
+          <t>objetivo_de_demanda</t>
         </is>
       </c>
       <c r="C80" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -1643,7 +1643,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>descripcion</t>
+          <t>estado_demanda</t>
         </is>
       </c>
       <c r="C81" t="b">
@@ -1658,11 +1658,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>objetivo_de_demanda</t>
+          <t>observaciones</t>
         </is>
       </c>
       <c r="C82" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>estado_demanda</t>
+          <t>envio_de_respuesta</t>
         </is>
       </c>
       <c r="C83" t="b">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>observaciones</t>
+          <t>etiqueta</t>
         </is>
       </c>
       <c r="C84" t="b">
@@ -1703,7 +1703,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>tipo_demanda</t>
+          <t>localizacion</t>
         </is>
       </c>
       <c r="C85" t="b">
@@ -1718,11 +1718,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>localizacion</t>
+          <t>ambito_vulneracion</t>
         </is>
       </c>
       <c r="C86" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -1733,11 +1733,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>ambito_vulneracion</t>
+          <t>bloque_datos_remitente</t>
         </is>
       </c>
       <c r="C87" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>tipos_presuntos_delitos</t>
+          <t>tipo_institucion</t>
         </is>
       </c>
       <c r="C88" t="b">
@@ -1763,11 +1763,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>bloque_datos_remitente</t>
+          <t>institucion</t>
         </is>
       </c>
       <c r="C89" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>tipo_institucion</t>
+          <t>motivo_ingreso</t>
         </is>
       </c>
       <c r="C90" t="b">
@@ -1793,7 +1793,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>institucion</t>
+          <t>submotivo_ingreso</t>
         </is>
       </c>
       <c r="C91" t="b">
@@ -1808,7 +1808,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>motivo_ingreso</t>
+          <t>registrado_por_user</t>
         </is>
       </c>
       <c r="C92" t="b">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>submotivo_ingreso</t>
+          <t>registrado_por_user_zona</t>
         </is>
       </c>
       <c r="C93" t="b">
@@ -1838,22 +1838,22 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>registrado_por_user</t>
+          <t>parent</t>
         </is>
       </c>
       <c r="C94" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>TDemandaHistory</t>
+          <t>TDemandaAdjunto</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>registrado_por_user_zona</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C95" t="b">
@@ -1863,16 +1863,16 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>TDemandaHistory</t>
+          <t>TDemandaAdjunto</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>parent</t>
+          <t>archivo</t>
         </is>
       </c>
       <c r="C96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>fecha</t>
         </is>
       </c>
       <c r="C97" t="b">
@@ -1898,22 +1898,22 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>archivo</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C98" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>TDemandaAdjunto</t>
+          <t>TTipoCodigoDemanda</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>fecha</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C99" t="b">
@@ -1923,12 +1923,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>TDemandaAdjunto</t>
+          <t>TTipoCodigoDemanda</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>nombre</t>
         </is>
       </c>
       <c r="C100" t="b">
@@ -1943,11 +1943,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>datatype</t>
         </is>
       </c>
       <c r="C101" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -1958,41 +1958,41 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>bloque_datos_remitente</t>
         </is>
       </c>
       <c r="C102" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>TTipoCodigoDemanda</t>
+          <t>TCodigoDemanda</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>datatype</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C103" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>TTipoCodigoDemanda</t>
+          <t>TCodigoDemanda</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>bloque_datos_remitente</t>
+          <t>codigo</t>
         </is>
       </c>
       <c r="C104" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -2003,11 +2003,11 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>tipo_codigo</t>
         </is>
       </c>
       <c r="C105" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106">
@@ -2018,7 +2018,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>codigo</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C106" t="b">
@@ -2028,31 +2028,31 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>TCodigoDemanda</t>
+          <t>TCalificacionDemanda</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>tipo_codigo</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C107" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>TCodigoDemanda</t>
+          <t>TCalificacionDemanda</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>fecha_y_hora_creacion</t>
         </is>
       </c>
       <c r="C108" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -2063,11 +2063,11 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>justificacion</t>
         </is>
       </c>
       <c r="C109" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -2078,11 +2078,11 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>fecha_y_hora_creacion</t>
+          <t>estado_calificacion</t>
         </is>
       </c>
       <c r="C110" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111">
@@ -2093,11 +2093,11 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>justificacion</t>
+          <t>ultima_actualizacion</t>
         </is>
       </c>
       <c r="C111" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112">
@@ -2108,7 +2108,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>estado_calificacion</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C112" t="b">
@@ -2118,12 +2118,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>TCalificacionDemanda</t>
+          <t>TCalificacionDemandaHistory</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>ultima_actualizacion</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C113" t="b">
@@ -2133,16 +2133,16 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>TCalificacionDemanda</t>
+          <t>TCalificacionDemandaHistory</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>descripcion</t>
         </is>
       </c>
       <c r="C114" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115">
@@ -2153,11 +2153,11 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>action</t>
         </is>
       </c>
       <c r="C115" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -2168,7 +2168,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>descripcion</t>
+          <t>by_user</t>
         </is>
       </c>
       <c r="C116" t="b">
@@ -2183,11 +2183,11 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>action</t>
+          <t>timestamp</t>
         </is>
       </c>
       <c r="C117" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>by_user</t>
+          <t>fecha_y_hora_creacion</t>
         </is>
       </c>
       <c r="C118" t="b">
@@ -2213,11 +2213,11 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>timestamp</t>
+          <t>justificacion</t>
         </is>
       </c>
       <c r="C119" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -2228,11 +2228,11 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>fecha_y_hora_creacion</t>
+          <t>estado_calificacion</t>
         </is>
       </c>
       <c r="C120" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -2243,11 +2243,11 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>justificacion</t>
+          <t>ultima_actualizacion</t>
         </is>
       </c>
       <c r="C121" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>estado_calificacion</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C122" t="b">
@@ -2273,41 +2273,41 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>ultima_actualizacion</t>
+          <t>parent</t>
         </is>
       </c>
       <c r="C123" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>TCalificacionDemandaHistory</t>
+          <t>TDemandaScore</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C124" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>TCalificacionDemandaHistory</t>
+          <t>TDemandaScore</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>parent</t>
+          <t>ultima_actualizacion</t>
         </is>
       </c>
       <c r="C125" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -2318,7 +2318,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>score</t>
         </is>
       </c>
       <c r="C126" t="b">
@@ -2333,7 +2333,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>ultima_actualizacion</t>
+          <t>score_condiciones_vulnerabilidad</t>
         </is>
       </c>
       <c r="C127" t="b">
@@ -2348,7 +2348,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>score</t>
+          <t>score_vulneracion</t>
         </is>
       </c>
       <c r="C128" t="b">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>score_condiciones_vulnerabilidad</t>
+          <t>score_motivos_intervencion</t>
         </is>
       </c>
       <c r="C129" t="b">
@@ -2378,7 +2378,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>score_vulneracion</t>
+          <t>score_indicadores_valoracion</t>
         </is>
       </c>
       <c r="C130" t="b">
@@ -2393,22 +2393,22 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>score_motivos_intervencion</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C131" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>TDemandaScore</t>
+          <t>TDemandaScoreHistory</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>score_indicadores_valoracion</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C132" t="b">
@@ -2418,16 +2418,16 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>TDemandaScore</t>
+          <t>TDemandaScoreHistory</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>descripcion</t>
         </is>
       </c>
       <c r="C133" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134">
@@ -2438,11 +2438,11 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>action</t>
         </is>
       </c>
       <c r="C134" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>descripcion</t>
+          <t>by_user</t>
         </is>
       </c>
       <c r="C135" t="b">
@@ -2468,11 +2468,11 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>action</t>
+          <t>timestamp</t>
         </is>
       </c>
       <c r="C136" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>by_user</t>
+          <t>ultima_actualizacion</t>
         </is>
       </c>
       <c r="C137" t="b">
@@ -2498,7 +2498,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>timestamp</t>
+          <t>score</t>
         </is>
       </c>
       <c r="C138" t="b">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>ultima_actualizacion</t>
+          <t>score_condiciones_vulnerabilidad</t>
         </is>
       </c>
       <c r="C139" t="b">
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>score</t>
+          <t>score_vulneracion</t>
         </is>
       </c>
       <c r="C140" t="b">
@@ -2543,7 +2543,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>score_condiciones_vulnerabilidad</t>
+          <t>score_motivos_intervencion</t>
         </is>
       </c>
       <c r="C141" t="b">
@@ -2558,7 +2558,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>score_vulneracion</t>
+          <t>score_indicadores_valoracion</t>
         </is>
       </c>
       <c r="C142" t="b">
@@ -2573,11 +2573,11 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>score_motivos_intervencion</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C143" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -2588,37 +2588,37 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>score_indicadores_valoracion</t>
+          <t>parent</t>
         </is>
       </c>
       <c r="C144" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>TDemandaScoreHistory</t>
+          <t>TVinculoDePersonas</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C145" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>TDemandaScoreHistory</t>
+          <t>TVinculoDePersonas</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>parent</t>
+          <t>nombre</t>
         </is>
       </c>
       <c r="C146" t="b">
@@ -2628,7 +2628,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>TVinculoDePersonas</t>
+          <t>TPersona</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -2643,16 +2643,16 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>TVinculoDePersonas</t>
+          <t>TPersona</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>deleted</t>
         </is>
       </c>
       <c r="C148" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149">
@@ -2663,11 +2663,11 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>nombre</t>
         </is>
       </c>
       <c r="C149" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150">
@@ -2678,7 +2678,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>deleted</t>
+          <t>nombre_autopercibido</t>
         </is>
       </c>
       <c r="C150" t="b">
@@ -2693,7 +2693,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>apellido</t>
         </is>
       </c>
       <c r="C151" t="b">
@@ -2708,7 +2708,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>nombre_autopercibido</t>
+          <t>fecha_nacimiento</t>
         </is>
       </c>
       <c r="C152" t="b">
@@ -2723,11 +2723,11 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>apellido</t>
+          <t>fecha_defuncion</t>
         </is>
       </c>
       <c r="C153" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154">
@@ -2738,7 +2738,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>fecha_nacimiento</t>
+          <t>edad_aproximada</t>
         </is>
       </c>
       <c r="C154" t="b">
@@ -2753,11 +2753,11 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>edad_aproximada</t>
+          <t>nacionalidad</t>
         </is>
       </c>
       <c r="C155" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156">
@@ -2768,11 +2768,11 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>nacionalidad</t>
+          <t>dni</t>
         </is>
       </c>
       <c r="C156" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
@@ -2783,11 +2783,11 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>dni</t>
+          <t>situacion_dni</t>
         </is>
       </c>
       <c r="C157" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>situacion_dni</t>
+          <t>genero</t>
         </is>
       </c>
       <c r="C158" t="b">
@@ -2813,11 +2813,11 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>genero</t>
+          <t>observaciones</t>
         </is>
       </c>
       <c r="C159" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160">
@@ -2828,11 +2828,11 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>observaciones</t>
+          <t>adulto</t>
         </is>
       </c>
       <c r="C160" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>adulto</t>
+          <t>nnya</t>
         </is>
       </c>
       <c r="C161" t="b">
@@ -2858,22 +2858,22 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>nnya</t>
+          <t>telefono</t>
         </is>
       </c>
       <c r="C162" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>TPersona</t>
+          <t>TPersonaHistory</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>telefono</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C163" t="b">
@@ -2888,7 +2888,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>descripcion</t>
         </is>
       </c>
       <c r="C164" t="b">
@@ -2903,11 +2903,11 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>descripcion</t>
+          <t>action</t>
         </is>
       </c>
       <c r="C165" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166">
@@ -2918,11 +2918,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>action</t>
+          <t>by_user</t>
         </is>
       </c>
       <c r="C166" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167">
@@ -2933,7 +2933,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>by_user</t>
+          <t>timestamp</t>
         </is>
       </c>
       <c r="C167" t="b">
@@ -2948,7 +2948,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>timestamp</t>
+          <t>deleted</t>
         </is>
       </c>
       <c r="C168" t="b">
@@ -2963,11 +2963,11 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>deleted</t>
+          <t>nombre</t>
         </is>
       </c>
       <c r="C169" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
@@ -2978,11 +2978,11 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>nombre_autopercibido</t>
         </is>
       </c>
       <c r="C170" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171">
@@ -2993,11 +2993,11 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>nombre_autopercibido</t>
+          <t>apellido</t>
         </is>
       </c>
       <c r="C171" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172">
@@ -3008,11 +3008,11 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>apellido</t>
+          <t>fecha_nacimiento</t>
         </is>
       </c>
       <c r="C172" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173">
@@ -3023,7 +3023,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>fecha_nacimiento</t>
+          <t>fecha_defuncion</t>
         </is>
       </c>
       <c r="C173" t="b">
@@ -6068,7 +6068,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>vinculo_demanda</t>
+          <t>legalmente_responsable</t>
         </is>
       </c>
       <c r="C376" t="b">
@@ -6083,7 +6083,7 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>vinculo_con_nnya_principal</t>
+          <t>ocupacion</t>
         </is>
       </c>
       <c r="C377" t="b">
@@ -6098,11 +6098,11 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>vinculo_demanda</t>
         </is>
       </c>
       <c r="C378" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="379">
@@ -6113,41 +6113,41 @@
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>persona</t>
+          <t>vinculo_con_nnya_principal</t>
         </is>
       </c>
       <c r="C379" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>TDemandaPersonaHistory</t>
+          <t>TDemandaPersona</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C380" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>TDemandaPersonaHistory</t>
+          <t>TDemandaPersona</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>descripcion</t>
+          <t>persona</t>
         </is>
       </c>
       <c r="C381" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="382">
@@ -6158,11 +6158,11 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>action</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C382" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="383">
@@ -6173,7 +6173,7 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>by_user</t>
+          <t>descripcion</t>
         </is>
       </c>
       <c r="C383" t="b">
@@ -6188,11 +6188,11 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>timestamp</t>
+          <t>action</t>
         </is>
       </c>
       <c r="C384" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="385">
@@ -6203,7 +6203,7 @@
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>deleted</t>
+          <t>by_user</t>
         </is>
       </c>
       <c r="C385" t="b">
@@ -6218,11 +6218,11 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>conviviente</t>
+          <t>timestamp</t>
         </is>
       </c>
       <c r="C386" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="387">
@@ -6233,7 +6233,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>vinculo_demanda</t>
+          <t>deleted</t>
         </is>
       </c>
       <c r="C387" t="b">
@@ -6248,11 +6248,11 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>vinculo_con_nnya_principal</t>
+          <t>conviviente</t>
         </is>
       </c>
       <c r="C388" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="389">
@@ -6263,11 +6263,11 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>legalmente_responsable</t>
         </is>
       </c>
       <c r="C389" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="390">
@@ -6278,11 +6278,11 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>persona</t>
+          <t>ocupacion</t>
         </is>
       </c>
       <c r="C390" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="391">
@@ -6293,22 +6293,22 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>parent</t>
+          <t>vinculo_demanda</t>
         </is>
       </c>
       <c r="C391" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>TDemandaZona</t>
+          <t>TDemandaPersonaHistory</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>vinculo_con_nnya_principal</t>
         </is>
       </c>
       <c r="C392" t="b">
@@ -6318,46 +6318,46 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>TDemandaZona</t>
+          <t>TDemandaPersonaHistory</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>esta_activo</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C393" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>TDemandaZona</t>
+          <t>TDemandaPersonaHistory</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>recibido</t>
+          <t>persona</t>
         </is>
       </c>
       <c r="C394" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>TDemandaZona</t>
+          <t>TDemandaPersonaHistory</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>comentarios</t>
+          <t>parent</t>
         </is>
       </c>
       <c r="C395" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="396">
@@ -6368,11 +6368,11 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C396" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="397">
@@ -6383,11 +6383,11 @@
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>zona</t>
+          <t>esta_activo</t>
         </is>
       </c>
       <c r="C397" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="398">
@@ -6398,7 +6398,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>user_responsable</t>
+          <t>recibido</t>
         </is>
       </c>
       <c r="C398" t="b">
@@ -6413,7 +6413,7 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>enviado_por</t>
+          <t>comentarios</t>
         </is>
       </c>
       <c r="C399" t="b">
@@ -6428,37 +6428,37 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>recibido_por</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C400" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>TDemandaZonaHistory</t>
+          <t>TDemandaZona</t>
         </is>
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>zona</t>
         </is>
       </c>
       <c r="C401" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>TDemandaZonaHistory</t>
+          <t>TDemandaZona</t>
         </is>
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>descripcion</t>
+          <t>user_responsable</t>
         </is>
       </c>
       <c r="C402" t="b">
@@ -6468,27 +6468,27 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>TDemandaZonaHistory</t>
+          <t>TDemandaZona</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>action</t>
+          <t>enviado_por</t>
         </is>
       </c>
       <c r="C403" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>TDemandaZonaHistory</t>
+          <t>TDemandaZona</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>by_user</t>
+          <t>recibido_por</t>
         </is>
       </c>
       <c r="C404" t="b">
@@ -6503,7 +6503,7 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>timestamp</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C405" t="b">
@@ -6518,7 +6518,7 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>esta_activo</t>
+          <t>descripcion</t>
         </is>
       </c>
       <c r="C406" t="b">
@@ -6533,11 +6533,11 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>recibido</t>
+          <t>action</t>
         </is>
       </c>
       <c r="C407" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="408">
@@ -6548,7 +6548,7 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>comentarios</t>
+          <t>by_user</t>
         </is>
       </c>
       <c r="C408" t="b">
@@ -6563,11 +6563,11 @@
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>timestamp</t>
         </is>
       </c>
       <c r="C409" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="410">
@@ -6578,11 +6578,11 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>zona</t>
+          <t>esta_activo</t>
         </is>
       </c>
       <c r="C410" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="411">
@@ -6593,7 +6593,7 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>user_responsable</t>
+          <t>recibido</t>
         </is>
       </c>
       <c r="C411" t="b">
@@ -6608,7 +6608,7 @@
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>enviado_por</t>
+          <t>comentarios</t>
         </is>
       </c>
       <c r="C412" t="b">
@@ -6623,11 +6623,11 @@
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>recibido_por</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C413" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="414">
@@ -6638,7 +6638,7 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>parent</t>
+          <t>zona</t>
         </is>
       </c>
       <c r="C414" t="b">
@@ -6648,12 +6648,12 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>TDemandaVinculada</t>
+          <t>TDemandaZonaHistory</t>
         </is>
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>user_responsable</t>
         </is>
       </c>
       <c r="C415" t="b">
@@ -6663,12 +6663,12 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>TDemandaVinculada</t>
+          <t>TDemandaZonaHistory</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>deleted</t>
+          <t>enviado_por</t>
         </is>
       </c>
       <c r="C416" t="b">
@@ -6678,27 +6678,27 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>TDemandaVinculada</t>
+          <t>TDemandaZonaHistory</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>demanda_1</t>
+          <t>recibido_por</t>
         </is>
       </c>
       <c r="C417" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>TDemandaVinculada</t>
+          <t>TDemandaZonaHistory</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>demanda_2</t>
+          <t>parent</t>
         </is>
       </c>
       <c r="C418" t="b">
@@ -6708,7 +6708,7 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>TDemandaVinculadaHistory</t>
+          <t>TDemandaVinculada</t>
         </is>
       </c>
       <c r="B419" t="inlineStr">
@@ -6723,12 +6723,12 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>TDemandaVinculadaHistory</t>
+          <t>TDemandaVinculada</t>
         </is>
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>descripcion</t>
+          <t>deleted</t>
         </is>
       </c>
       <c r="C420" t="b">
@@ -6738,12 +6738,12 @@
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>TDemandaVinculadaHistory</t>
+          <t>TDemandaVinculada</t>
         </is>
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>action</t>
+          <t>demanda_1</t>
         </is>
       </c>
       <c r="C421" t="b">
@@ -6753,16 +6753,16 @@
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>TDemandaVinculadaHistory</t>
+          <t>TDemandaVinculada</t>
         </is>
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>by_user</t>
+          <t>demanda_2</t>
         </is>
       </c>
       <c r="C422" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="423">
@@ -6773,7 +6773,7 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>timestamp</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C423" t="b">
@@ -6788,7 +6788,7 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>deleted</t>
+          <t>descripcion</t>
         </is>
       </c>
       <c r="C424" t="b">
@@ -6803,7 +6803,7 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>demanda_1</t>
+          <t>action</t>
         </is>
       </c>
       <c r="C425" t="b">
@@ -6818,11 +6818,11 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>demanda_2</t>
+          <t>by_user</t>
         </is>
       </c>
       <c r="C426" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="427">
@@ -6833,22 +6833,22 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>parent</t>
+          <t>timestamp</t>
         </is>
       </c>
       <c r="C427" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>TPersonaCondicionesVulnerabilidad</t>
+          <t>TDemandaVinculadaHistory</t>
         </is>
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>deleted</t>
         </is>
       </c>
       <c r="C428" t="b">
@@ -6858,12 +6858,12 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>TPersonaCondicionesVulnerabilidad</t>
+          <t>TDemandaVinculadaHistory</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>si_no</t>
+          <t>demanda_1</t>
         </is>
       </c>
       <c r="C429" t="b">
@@ -6873,12 +6873,12 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>TPersonaCondicionesVulnerabilidad</t>
+          <t>TDemandaVinculadaHistory</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>persona</t>
+          <t>demanda_2</t>
         </is>
       </c>
       <c r="C430" t="b">
@@ -6888,12 +6888,12 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>TPersonaCondicionesVulnerabilidad</t>
+          <t>TDemandaVinculadaHistory</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>condicion_vulnerabilidad</t>
+          <t>parent</t>
         </is>
       </c>
       <c r="C431" t="b">
@@ -6908,7 +6908,7 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C432" t="b">
@@ -6918,42 +6918,42 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>TPersonaCondicionesVulnerabilidadHistory</t>
+          <t>TPersonaCondicionesVulnerabilidad</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>si_no</t>
         </is>
       </c>
       <c r="C433" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>TPersonaCondicionesVulnerabilidadHistory</t>
+          <t>TPersonaCondicionesVulnerabilidad</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>descripcion</t>
+          <t>persona</t>
         </is>
       </c>
       <c r="C434" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>TPersonaCondicionesVulnerabilidadHistory</t>
+          <t>TPersonaCondicionesVulnerabilidad</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>action</t>
+          <t>condicion_vulnerabilidad</t>
         </is>
       </c>
       <c r="C435" t="b">
@@ -6963,12 +6963,12 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>TPersonaCondicionesVulnerabilidadHistory</t>
+          <t>TPersonaCondicionesVulnerabilidad</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>by_user</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C436" t="b">
@@ -6983,7 +6983,7 @@
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>timestamp</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C437" t="b">
@@ -6998,11 +6998,11 @@
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>si_no</t>
+          <t>descripcion</t>
         </is>
       </c>
       <c r="C438" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="439">
@@ -7013,7 +7013,7 @@
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>persona</t>
+          <t>action</t>
         </is>
       </c>
       <c r="C439" t="b">
@@ -7028,11 +7028,11 @@
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>condicion_vulnerabilidad</t>
+          <t>by_user</t>
         </is>
       </c>
       <c r="C440" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="441">
@@ -7043,7 +7043,7 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>timestamp</t>
         </is>
       </c>
       <c r="C441" t="b">
@@ -7058,7 +7058,7 @@
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>parent</t>
+          <t>si_no</t>
         </is>
       </c>
       <c r="C442" t="b">
@@ -7068,27 +7068,27 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>TActividadTipo</t>
+          <t>TPersonaCondicionesVulnerabilidadHistory</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>persona</t>
         </is>
       </c>
       <c r="C443" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>TActividadTipo</t>
+          <t>TPersonaCondicionesVulnerabilidadHistory</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>condicion_vulnerabilidad</t>
         </is>
       </c>
       <c r="C444" t="b">
@@ -7098,12 +7098,12 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>TActividadTipo</t>
+          <t>TPersonaCondicionesVulnerabilidadHistory</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>remitir_a_jefe</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C445" t="b">
@@ -7113,27 +7113,27 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>TActividadTipoModelo</t>
+          <t>TPersonaCondicionesVulnerabilidadHistory</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>parent</t>
         </is>
       </c>
       <c r="C446" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>TActividadTipoModelo</t>
+          <t>TActividadTipo</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>archivo</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C447" t="b">
@@ -7143,37 +7143,37 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>TActividadTipoModelo</t>
+          <t>TActividadTipo</t>
         </is>
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>fecha</t>
+          <t>nombre</t>
         </is>
       </c>
       <c r="C448" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>TActividadTipoModelo</t>
+          <t>TActividadTipo</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>actividad_tipo</t>
+          <t>remitir_a_jefe</t>
         </is>
       </c>
       <c r="C449" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>TInstitucionActividad</t>
+          <t>TActividadTipoModelo</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
@@ -7188,27 +7188,27 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>TInstitucionActividad</t>
+          <t>TActividadTipoModelo</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>archivo</t>
         </is>
       </c>
       <c r="C451" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>TActividad</t>
+          <t>TActividadTipoModelo</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>fecha</t>
         </is>
       </c>
       <c r="C452" t="b">
@@ -7218,42 +7218,42 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>TActividad</t>
+          <t>TActividadTipoModelo</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>fecha_y_hora</t>
+          <t>actividad_tipo</t>
         </is>
       </c>
       <c r="C453" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>TActividad</t>
+          <t>TInstitucionActividad</t>
         </is>
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>fecha_y_hora_manual</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C454" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>TActividad</t>
+          <t>TInstitucionActividad</t>
         </is>
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>descripcion</t>
+          <t>nombre</t>
         </is>
       </c>
       <c r="C455" t="b">
@@ -7268,11 +7268,11 @@
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C456" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="457">
@@ -7283,7 +7283,7 @@
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>tipo</t>
+          <t>fecha_y_hora</t>
         </is>
       </c>
       <c r="C457" t="b">
@@ -7298,37 +7298,37 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>institucion</t>
+          <t>fecha_y_hora_manual</t>
         </is>
       </c>
       <c r="C458" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>TActividadHistory</t>
+          <t>TActividad</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>descripcion</t>
         </is>
       </c>
       <c r="C459" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>TActividadHistory</t>
+          <t>TActividad</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>action</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C460" t="b">
@@ -7338,12 +7338,12 @@
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>TActividadHistory</t>
+          <t>TActividad</t>
         </is>
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>by_user</t>
+          <t>tipo</t>
         </is>
       </c>
       <c r="C461" t="b">
@@ -7353,12 +7353,12 @@
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>TActividadHistory</t>
+          <t>TActividad</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>timestamp</t>
+          <t>institucion</t>
         </is>
       </c>
       <c r="C462" t="b">
@@ -7368,12 +7368,12 @@
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>TActividadHistory</t>
+          <t>TActividad</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>fecha_y_hora</t>
+          <t>by_user</t>
         </is>
       </c>
       <c r="C463" t="b">
@@ -7383,72 +7383,72 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>TActividadHistory</t>
+          <t>TActividadAdjunto</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>fecha_y_hora_manual</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C464" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>TActividadHistory</t>
+          <t>TActividadAdjunto</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>descripcion</t>
+          <t>archivo</t>
         </is>
       </c>
       <c r="C465" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>TActividadHistory</t>
+          <t>TActividadAdjunto</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>fecha</t>
         </is>
       </c>
       <c r="C466" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>TActividadHistory</t>
+          <t>TActividadAdjunto</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>tipo</t>
+          <t>actividad</t>
         </is>
       </c>
       <c r="C467" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>TActividadHistory</t>
+          <t>TRespuestaEtiqueta</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>institucion</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C468" t="b">
@@ -7458,12 +7458,12 @@
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>TActividadHistory</t>
+          <t>TRespuestaEtiqueta</t>
         </is>
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>parent</t>
+          <t>nombre</t>
         </is>
       </c>
       <c r="C469" t="b">
@@ -7473,7 +7473,7 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>TActividadAdjunto</t>
+          <t>TRespuesta</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
@@ -7488,12 +7488,12 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>TActividadAdjunto</t>
+          <t>TRespuesta</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>archivo</t>
+          <t>fecha_y_hora</t>
         </is>
       </c>
       <c r="C471" t="b">
@@ -7503,12 +7503,12 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>TActividadAdjunto</t>
+          <t>TRespuesta</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>fecha</t>
+          <t>cc</t>
         </is>
       </c>
       <c r="C472" t="b">
@@ -7518,27 +7518,27 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>TActividadAdjunto</t>
+          <t>TRespuesta</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>actividad</t>
+          <t>bcc</t>
         </is>
       </c>
       <c r="C473" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>TRespuestaEtiqueta</t>
+          <t>TRespuesta</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>to</t>
         </is>
       </c>
       <c r="C474" t="b">
@@ -7548,12 +7548,12 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>TRespuestaEtiqueta</t>
+          <t>TRespuesta</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>asunto</t>
         </is>
       </c>
       <c r="C475" t="b">
@@ -7568,11 +7568,11 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>mensaje</t>
         </is>
       </c>
       <c r="C476" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="477">
@@ -7583,11 +7583,11 @@
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>fecha_y_hora</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C477" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="478">
@@ -7598,11 +7598,11 @@
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>cc</t>
+          <t>institucion</t>
         </is>
       </c>
       <c r="C478" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="479">
@@ -7613,7 +7613,7 @@
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>bcc</t>
+          <t>by_user</t>
         </is>
       </c>
       <c r="C479" t="b">
@@ -7628,7 +7628,7 @@
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>to</t>
+          <t>etiqueta</t>
         </is>
       </c>
       <c r="C480" t="b">
@@ -7638,57 +7638,57 @@
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>TRespuesta</t>
+          <t>TRespuestaAdjunto</t>
         </is>
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>asunto</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C481" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>TRespuesta</t>
+          <t>TRespuestaAdjunto</t>
         </is>
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>mensaje</t>
+          <t>archivo</t>
         </is>
       </c>
       <c r="C482" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>TRespuesta</t>
+          <t>TRespuestaAdjunto</t>
         </is>
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>fecha</t>
         </is>
       </c>
       <c r="C483" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>TRespuesta</t>
+          <t>TRespuestaAdjunto</t>
         </is>
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>institucion</t>
+          <t>respuesta</t>
         </is>
       </c>
       <c r="C484" t="b">
@@ -7698,12 +7698,12 @@
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>TRespuesta</t>
+          <t>TIndicadoresValoracion</t>
         </is>
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>etiqueta</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C485" t="b">
@@ -7713,27 +7713,27 @@
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>TRespuestaAdjunto</t>
+          <t>TIndicadoresValoracion</t>
         </is>
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>nombre</t>
         </is>
       </c>
       <c r="C486" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>TRespuestaAdjunto</t>
+          <t>TIndicadoresValoracion</t>
         </is>
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>archivo</t>
+          <t>descripcion</t>
         </is>
       </c>
       <c r="C487" t="b">
@@ -7743,12 +7743,12 @@
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>TRespuestaAdjunto</t>
+          <t>TIndicadoresValoracion</t>
         </is>
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>fecha</t>
+          <t>peso</t>
         </is>
       </c>
       <c r="C488" t="b">
@@ -7758,42 +7758,42 @@
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>TRespuestaAdjunto</t>
+          <t>TEvaluaciones</t>
         </is>
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>respuesta</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C489" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>TIndicadoresValoracion</t>
+          <t>TEvaluaciones</t>
         </is>
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C490" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t>TIndicadoresValoracion</t>
+          <t>TEvaluaciones</t>
         </is>
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>indicador</t>
         </is>
       </c>
       <c r="C491" t="b">
@@ -7803,27 +7803,27 @@
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t>TIndicadoresValoracion</t>
+          <t>TEvaluaciones</t>
         </is>
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>descripcion</t>
+          <t>si_no</t>
         </is>
       </c>
       <c r="C492" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>TIndicadoresValoracion</t>
+          <t>TEvaluacionesHistory</t>
         </is>
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>peso</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C493" t="b">
@@ -7833,12 +7833,12 @@
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>TEvaluaciones</t>
+          <t>TEvaluacionesHistory</t>
         </is>
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>descripcion</t>
         </is>
       </c>
       <c r="C494" t="b">
@@ -7848,12 +7848,12 @@
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>TEvaluaciones</t>
+          <t>TEvaluacionesHistory</t>
         </is>
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>action</t>
         </is>
       </c>
       <c r="C495" t="b">
@@ -7863,31 +7863,31 @@
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>TEvaluaciones</t>
+          <t>TEvaluacionesHistory</t>
         </is>
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>indicador</t>
+          <t>by_user</t>
         </is>
       </c>
       <c r="C496" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t>TEvaluaciones</t>
+          <t>TEvaluacionesHistory</t>
         </is>
       </c>
       <c r="B497" t="inlineStr">
         <is>
-          <t>si_no</t>
+          <t>timestamp</t>
         </is>
       </c>
       <c r="C497" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="498">
@@ -7898,11 +7898,11 @@
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C498" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="499">
@@ -7913,11 +7913,11 @@
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>descripcion</t>
+          <t>indicador</t>
         </is>
       </c>
       <c r="C499" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="500">
@@ -7928,7 +7928,7 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>action</t>
+          <t>si_no</t>
         </is>
       </c>
       <c r="C500" t="b">
@@ -7943,22 +7943,22 @@
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>by_user</t>
+          <t>parent</t>
         </is>
       </c>
       <c r="C501" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="502">
       <c r="A502" t="inlineStr">
         <is>
-          <t>TEvaluacionesHistory</t>
+          <t>TDecision</t>
         </is>
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>timestamp</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C502" t="b">
@@ -7968,27 +7968,27 @@
     <row r="503">
       <c r="A503" t="inlineStr">
         <is>
-          <t>TEvaluacionesHistory</t>
+          <t>TDecision</t>
         </is>
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>fecha_y_hora</t>
         </is>
       </c>
       <c r="C503" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="504">
       <c r="A504" t="inlineStr">
         <is>
-          <t>TEvaluacionesHistory</t>
+          <t>TDecision</t>
         </is>
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>indicador</t>
+          <t>justificacion</t>
         </is>
       </c>
       <c r="C504" t="b">
@@ -7998,12 +7998,12 @@
     <row r="505">
       <c r="A505" t="inlineStr">
         <is>
-          <t>TEvaluacionesHistory</t>
+          <t>TDecision</t>
         </is>
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>si_no</t>
+          <t>decision</t>
         </is>
       </c>
       <c r="C505" t="b">
@@ -8013,12 +8013,12 @@
     <row r="506">
       <c r="A506" t="inlineStr">
         <is>
-          <t>TEvaluacionesHistory</t>
+          <t>TDecision</t>
         </is>
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>parent</t>
+          <t>demanda</t>
         </is>
       </c>
       <c r="C506" t="b">
@@ -8033,22 +8033,22 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>nnya</t>
         </is>
       </c>
       <c r="C507" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="508">
       <c r="A508" t="inlineStr">
         <is>
-          <t>TDecision</t>
+          <t>ValidacionConfiguracion</t>
         </is>
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>fecha_y_hora</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C508" t="b">
@@ -8058,61 +8058,61 @@
     <row r="509">
       <c r="A509" t="inlineStr">
         <is>
-          <t>TDecision</t>
+          <t>ValidacionConfiguracion</t>
         </is>
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>justificacion</t>
+          <t>required_fields</t>
         </is>
       </c>
       <c r="C509" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="510">
       <c r="A510" t="inlineStr">
         <is>
-          <t>TDecision</t>
+          <t>ValidacionConfiguracion</t>
         </is>
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>decision</t>
+          <t>required_activity_types</t>
         </is>
       </c>
       <c r="C510" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="511">
       <c r="A511" t="inlineStr">
         <is>
-          <t>TDecision</t>
+          <t>ValidacionConfiguracion</t>
         </is>
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>demanda</t>
+          <t>required_response_types</t>
         </is>
       </c>
       <c r="C511" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="512">
       <c r="A512" t="inlineStr">
         <is>
-          <t>TDecision</t>
+          <t>ValidacionConfiguracion</t>
         </is>
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>nnya</t>
+          <t>activo</t>
         </is>
       </c>
       <c r="C512" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>